<commit_message>
Added Alpha sheet to excel files
</commit_message>
<xml_diff>
--- a/src/mappings/mobile/xlsx/veris-1_3_7-mappings-mobile_v12.xlsx
+++ b/src/mappings/mobile/xlsx/veris-1_3_7-mappings-mobile_v12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitre-my.sharepoint.com/personal/javoss_mitre_org/Documents/Documents/Veris II/veris-2/src/mappings/mobile/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="6_{ACAA37AD-42AF-4D02-A299-4CDD764FD86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F0DA90D-66DB-4132-855F-A284FBC621B3}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="6_{ACAA37AD-42AF-4D02-A299-4CDD764FD86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E07D8B9-9E78-4B30-A1C2-9CC372875EE8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="11" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="8" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="498">
   <si>
     <t>ATT&amp;CK Integration into VERIS</t>
   </si>
@@ -1346,6 +1346,201 @@
   </si>
   <si>
     <t>Hijack</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Abuse of functionality</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Exploit misconfig</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Client-side attack</t>
+  </si>
+  <si>
+    <t>attribute.availability.variety.Destruction</t>
+  </si>
+  <si>
+    <t>attribute.availability.variety.Interruption</t>
+  </si>
+  <si>
+    <t>attribute.integrity.variety.Modify configuration</t>
+  </si>
+  <si>
+    <t>action.hacking.vector.Backdoor</t>
+  </si>
+  <si>
+    <t>action.malware.variety.C2</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Modify data</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Backdoor or C2</t>
+  </si>
+  <si>
+    <t>attribute.integrity.variety.Modify privileges</t>
+  </si>
+  <si>
+    <t>action.hacking.vector.Command shell</t>
+  </si>
+  <si>
+    <t>value_chain.distribution.variety.Phone</t>
+  </si>
+  <si>
+    <t>attribute.integrity.variety.Alter behavior</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Capture stored data</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Backdoor</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.DoS</t>
+  </si>
+  <si>
+    <t>action.malware.variety.DoS</t>
+  </si>
+  <si>
+    <t>attribute.availability.variety.Degradation</t>
+  </si>
+  <si>
+    <t>attribute.availability.variety.Loss</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Evade Defenses</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Profile host</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Evade Defenses</t>
+  </si>
+  <si>
+    <t>action.social.variety.Evade Defenses</t>
+  </si>
+  <si>
+    <t>attribute.integrity.variety.Log tampering</t>
+  </si>
+  <si>
+    <t>attribute.integrity.variety.Modify data</t>
+  </si>
+  <si>
+    <t>attribute.availability.variety.Obscuration</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Exploit vuln</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Fuzz testing</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Exploit vuln</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Hijack</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Unknown</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Use of stolen creds</t>
+  </si>
+  <si>
+    <t>action.malware.variety.MitM</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.MitM</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Scan network</t>
+  </si>
+  <si>
+    <t>action.hacking.variety.Other</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Backdoor</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Trojan</t>
+  </si>
+  <si>
+    <t>action.hacking.vector.Partner</t>
+  </si>
+  <si>
+    <t>action.social.vector.Software</t>
+  </si>
+  <si>
+    <t>action.social.vector.Phone</t>
+  </si>
+  <si>
+    <t>attribute.integrity.variety.Hardware tampering</t>
+  </si>
+  <si>
+    <t>action.hacking.vector.Other network service</t>
+  </si>
+  <si>
+    <t>attribute.integrity.variety.Misrepresentation</t>
+  </si>
+  <si>
+    <t>value_chain.non-distribution services.variety.Proxy</t>
+  </si>
+  <si>
+    <t>action.malware.vector.Instant messaging</t>
+  </si>
+  <si>
+    <t>action.social.variety.Pretexting</t>
+  </si>
+  <si>
+    <t>action.social.vector.SMS</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Capture app data</t>
+  </si>
+  <si>
+    <t>action.social.vector.Email</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Disable controls</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Export data</t>
+  </si>
+  <si>
+    <t>action.malware.variety.In-memory</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Ransomware</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Spyware/Keylogger</t>
+  </si>
+  <si>
+    <t>action.malware.variety.Worm</t>
+  </si>
+  <si>
+    <t>action.malware.vector.Removable media</t>
+  </si>
+  <si>
+    <t>action.social.vector.Removable media</t>
+  </si>
+  <si>
+    <t>action.malware.vector.Software update</t>
+  </si>
+  <si>
+    <t>attribute.integrity.variety.Software installation</t>
+  </si>
+  <si>
+    <t>action.malware.vector.Web application - drive-by</t>
+  </si>
+  <si>
+    <t>action.social.vector.Web application</t>
+  </si>
+  <si>
+    <t>action.social.vector.In-person</t>
+  </si>
+  <si>
+    <t>value_chain.targeting.variety.Lost or stolen credentials</t>
   </si>
 </sst>
 </file>
@@ -1623,6 +1818,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2690,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B670464-1153-4AA6-978E-5B7FAB2C4B98}">
   <dimension ref="A1:C314"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2710,6 +2909,2622 @@
       </c>
       <c r="C1" s="39" t="s">
         <v>431</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1626/","T1626")</f>
+        <v>T1626</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1626/","T1626")</f>
+        <v>T1626</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1626/","T1626")</f>
+        <v>T1626</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1626/001/","T1626.001")</f>
+        <v>T1626.001</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1626/001/","T1626.001")</f>
+        <v>T1626.001</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1640/","T1640")</f>
+        <v>T1640</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1640/","T1640")</f>
+        <v>T1640</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1640/","T1640")</f>
+        <v>T1640</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1640/","T1640")</f>
+        <v>T1640</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1437/","T1437")</f>
+        <v>T1437</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1437/","T1437")</f>
+        <v>T1437</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1437/","T1437")</f>
+        <v>T1437</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1532/","T1532")</f>
+        <v>T1532</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1532/","T1532")</f>
+        <v>T1532</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1398/","T1398")</f>
+        <v>T1398</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1398/","T1398")</f>
+        <v>T1398</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1398/","T1398")</f>
+        <v>T1398</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1398/","T1398")</f>
+        <v>T1398</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1398/","T1398")</f>
+        <v>T1398</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1623/","T1623")</f>
+        <v>T1623</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1623/","T1623")</f>
+        <v>T1623</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1623/","T1623")</f>
+        <v>T1623</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1623/001/","T1623.001")</f>
+        <v>T1623.001</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1623/001/","T1623.001")</f>
+        <v>T1623.001</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1623/001/","T1623.001")</f>
+        <v>T1623.001</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1624/","T1624")</f>
+        <v>T1624</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1624/","T1624")</f>
+        <v>T1624</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1624/001/","T1624.001")</f>
+        <v>T1624.001</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1624/001/","T1624.001")</f>
+        <v>T1624.001</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1636/","T1636")</f>
+        <v>T1636</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1636/","T1636")</f>
+        <v>T1636</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1636/001/","T1636.001")</f>
+        <v>T1636.001</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1636/001/","T1636.001")</f>
+        <v>T1636.001</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1636/002/","T1636.002")</f>
+        <v>T1636.002</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1636/002/","T1636.002")</f>
+        <v>T1636.002</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1636/003/","T1636.003")</f>
+        <v>T1636.003</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1636/003/","T1636.003")</f>
+        <v>T1636.003</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1636/004/","T1636.004")</f>
+        <v>T1636.004</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1636/004/","T1636.004")</f>
+        <v>T1636.004</v>
+      </c>
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1603/","T1603")</f>
+        <v>T1603</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1603/","T1603")</f>
+        <v>T1603</v>
+      </c>
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1541/","T1541")</f>
+        <v>T1541</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1629/001/","T1629.001")</f>
+        <v>T1629.001</v>
+      </c>
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1629/002/","T1629.002")</f>
+        <v>T1629.002</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1629/002/","T1629.002")</f>
+        <v>T1629.002</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1629/002/","T1629.002")</f>
+        <v>T1629.002</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1521/","T1521")</f>
+        <v>T1521</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1521/","T1521")</f>
+        <v>T1521</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1521/001/","T1521.001")</f>
+        <v>T1521.001</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1521/001/","T1521.001")</f>
+        <v>T1521.001</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1521/002/","T1521.002")</f>
+        <v>T1521.002</v>
+      </c>
+      <c r="B52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1521/002/","T1521.002")</f>
+        <v>T1521.002</v>
+      </c>
+      <c r="B53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1642/","T1642")</f>
+        <v>T1642</v>
+      </c>
+      <c r="B54" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1642/","T1642")</f>
+        <v>T1642</v>
+      </c>
+      <c r="B55" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1642/","T1642")</f>
+        <v>T1642</v>
+      </c>
+      <c r="B56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1642/","T1642")</f>
+        <v>T1642</v>
+      </c>
+      <c r="B57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1464/","T1464")</f>
+        <v>T1464</v>
+      </c>
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1464/","T1464")</f>
+        <v>T1464</v>
+      </c>
+      <c r="B59" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1464/","T1464")</f>
+        <v>T1464</v>
+      </c>
+      <c r="B60" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1464/","T1464")</f>
+        <v>T1464</v>
+      </c>
+      <c r="B61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1627/","T1627")</f>
+        <v>T1627</v>
+      </c>
+      <c r="B62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1627/","T1627")</f>
+        <v>T1627</v>
+      </c>
+      <c r="B63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1627/","T1627")</f>
+        <v>T1627</v>
+      </c>
+      <c r="B64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1627/","T1627")</f>
+        <v>T1627</v>
+      </c>
+      <c r="B65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1627/001/","T1627.001")</f>
+        <v>T1627.001</v>
+      </c>
+      <c r="B66" t="s">
+        <v>73</v>
+      </c>
+      <c r="C66" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1627/001/","T1627.001")</f>
+        <v>T1627.001</v>
+      </c>
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1627/001/","T1627.001")</f>
+        <v>T1627.001</v>
+      </c>
+      <c r="B68" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1627/001/","T1627.001")</f>
+        <v>T1627.001</v>
+      </c>
+      <c r="B69" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1628/","T1628")</f>
+        <v>T1628</v>
+      </c>
+      <c r="B70" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1628/","T1628")</f>
+        <v>T1628</v>
+      </c>
+      <c r="B71" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1628/","T1628")</f>
+        <v>T1628</v>
+      </c>
+      <c r="B72" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1628/001/","T1628.001")</f>
+        <v>T1628.001</v>
+      </c>
+      <c r="B73" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1628/001/","T1628.001")</f>
+        <v>T1628.001</v>
+      </c>
+      <c r="B74" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1628/001/","T1628.001")</f>
+        <v>T1628.001</v>
+      </c>
+      <c r="B75" t="s">
+        <v>77</v>
+      </c>
+      <c r="C75" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1628/002/","T1628.002")</f>
+        <v>T1628.002</v>
+      </c>
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1628/002/","T1628.002")</f>
+        <v>T1628.002</v>
+      </c>
+      <c r="B77" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1628/002/","T1628.002")</f>
+        <v>T1628.002</v>
+      </c>
+      <c r="B78" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/","T1630")</f>
+        <v>T1630</v>
+      </c>
+      <c r="B79" t="s">
+        <v>81</v>
+      </c>
+      <c r="C79" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/","T1630")</f>
+        <v>T1630</v>
+      </c>
+      <c r="B80" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/","T1630")</f>
+        <v>T1630</v>
+      </c>
+      <c r="B81" t="s">
+        <v>81</v>
+      </c>
+      <c r="C81" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/","T1630")</f>
+        <v>T1630</v>
+      </c>
+      <c r="B82" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/","T1630")</f>
+        <v>T1630</v>
+      </c>
+      <c r="B83" t="s">
+        <v>81</v>
+      </c>
+      <c r="C83" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/","T1406")</f>
+        <v>T1406</v>
+      </c>
+      <c r="B84" t="s">
+        <v>83</v>
+      </c>
+      <c r="C84" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/","T1406")</f>
+        <v>T1406</v>
+      </c>
+      <c r="B85" t="s">
+        <v>83</v>
+      </c>
+      <c r="C85" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/","T1406")</f>
+        <v>T1406</v>
+      </c>
+      <c r="B86" t="s">
+        <v>83</v>
+      </c>
+      <c r="C86" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/","T1406")</f>
+        <v>T1406</v>
+      </c>
+      <c r="B87" t="s">
+        <v>83</v>
+      </c>
+      <c r="C87" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/001/","T1406.001")</f>
+        <v>T1406.001</v>
+      </c>
+      <c r="B88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C88" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/001/","T1406.001")</f>
+        <v>T1406.001</v>
+      </c>
+      <c r="B89" t="s">
+        <v>85</v>
+      </c>
+      <c r="C89" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/001/","T1406.001")</f>
+        <v>T1406.001</v>
+      </c>
+      <c r="B90" t="s">
+        <v>85</v>
+      </c>
+      <c r="C90" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/001/","T1406.001")</f>
+        <v>T1406.001</v>
+      </c>
+      <c r="B91" t="s">
+        <v>85</v>
+      </c>
+      <c r="C91" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/002/","T1406.002")</f>
+        <v>T1406.002</v>
+      </c>
+      <c r="B92" t="s">
+        <v>87</v>
+      </c>
+      <c r="C92" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/002/","T1406.002")</f>
+        <v>T1406.002</v>
+      </c>
+      <c r="B93" t="s">
+        <v>87</v>
+      </c>
+      <c r="C93" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/002/","T1406.002")</f>
+        <v>T1406.002</v>
+      </c>
+      <c r="B94" t="s">
+        <v>87</v>
+      </c>
+      <c r="C94" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1406/002/","T1406.002")</f>
+        <v>T1406.002</v>
+      </c>
+      <c r="B95" t="s">
+        <v>87</v>
+      </c>
+      <c r="C95" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1644/","T1644")</f>
+        <v>T1644</v>
+      </c>
+      <c r="B96" t="s">
+        <v>89</v>
+      </c>
+      <c r="C96" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1644/","T1644")</f>
+        <v>T1644</v>
+      </c>
+      <c r="B97" t="s">
+        <v>89</v>
+      </c>
+      <c r="C97" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1644/","T1644")</f>
+        <v>T1644</v>
+      </c>
+      <c r="B98" t="s">
+        <v>89</v>
+      </c>
+      <c r="C98" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1644/","T1644")</f>
+        <v>T1644</v>
+      </c>
+      <c r="B99" t="s">
+        <v>89</v>
+      </c>
+      <c r="C99" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1644/","T1644")</f>
+        <v>T1644</v>
+      </c>
+      <c r="B100" t="s">
+        <v>89</v>
+      </c>
+      <c r="C100" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1404/","T1404")</f>
+        <v>T1404</v>
+      </c>
+      <c r="B101" t="s">
+        <v>92</v>
+      </c>
+      <c r="C101" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1404/","T1404")</f>
+        <v>T1404</v>
+      </c>
+      <c r="B102" t="s">
+        <v>92</v>
+      </c>
+      <c r="C102" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1404/","T1404")</f>
+        <v>T1404</v>
+      </c>
+      <c r="B103" t="s">
+        <v>92</v>
+      </c>
+      <c r="C103" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1428/","T1428")</f>
+        <v>T1428</v>
+      </c>
+      <c r="B104" t="s">
+        <v>94</v>
+      </c>
+      <c r="C104" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1428/","T1428")</f>
+        <v>T1428</v>
+      </c>
+      <c r="B105" t="s">
+        <v>94</v>
+      </c>
+      <c r="C105" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1625/","T1625")</f>
+        <v>T1625</v>
+      </c>
+      <c r="B106" t="s">
+        <v>100</v>
+      </c>
+      <c r="C106" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A107" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1625/","T1625")</f>
+        <v>T1625</v>
+      </c>
+      <c r="B107" t="s">
+        <v>100</v>
+      </c>
+      <c r="C107" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A108" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1625/001/","T1625.001")</f>
+        <v>T1625.001</v>
+      </c>
+      <c r="B108" t="s">
+        <v>102</v>
+      </c>
+      <c r="C108" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A109" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1625/001/","T1625.001")</f>
+        <v>T1625.001</v>
+      </c>
+      <c r="B109" t="s">
+        <v>102</v>
+      </c>
+      <c r="C109" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1635/001/","T1635.001")</f>
+        <v>T1635.001</v>
+      </c>
+      <c r="B110" t="s">
+        <v>104</v>
+      </c>
+      <c r="C110" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1635/001/","T1635.001")</f>
+        <v>T1635.001</v>
+      </c>
+      <c r="B111" t="s">
+        <v>104</v>
+      </c>
+      <c r="C111" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A112" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1635/001/","T1635.001")</f>
+        <v>T1635.001</v>
+      </c>
+      <c r="B112" t="s">
+        <v>104</v>
+      </c>
+      <c r="C112" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A113" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1638/","T1638")</f>
+        <v>T1638</v>
+      </c>
+      <c r="B113" t="s">
+        <v>115</v>
+      </c>
+      <c r="C113" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A114" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1426/","T1426")</f>
+        <v>T1426</v>
+      </c>
+      <c r="B114" t="s">
+        <v>122</v>
+      </c>
+      <c r="C114" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A115" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1418/","T1418")</f>
+        <v>T1418</v>
+      </c>
+      <c r="B115" t="s">
+        <v>124</v>
+      </c>
+      <c r="C115" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A116" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1418/001/","T1418.001")</f>
+        <v>T1418.001</v>
+      </c>
+      <c r="B116" t="s">
+        <v>126</v>
+      </c>
+      <c r="C116" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A117" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1424/","T1424")</f>
+        <v>T1424</v>
+      </c>
+      <c r="B117" t="s">
+        <v>129</v>
+      </c>
+      <c r="C117" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A118" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1422/","T1422")</f>
+        <v>T1422</v>
+      </c>
+      <c r="B118" t="s">
+        <v>135</v>
+      </c>
+      <c r="C118" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A119" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1421/","T1421")</f>
+        <v>T1421</v>
+      </c>
+      <c r="B119" t="s">
+        <v>137</v>
+      </c>
+      <c r="C119" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A120" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1423/","T1423")</f>
+        <v>T1423</v>
+      </c>
+      <c r="B120" t="s">
+        <v>139</v>
+      </c>
+      <c r="C120" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A121" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1631/","T1631")</f>
+        <v>T1631</v>
+      </c>
+      <c r="B121" t="s">
+        <v>161</v>
+      </c>
+      <c r="C121" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A122" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1631/001/","T1631.001")</f>
+        <v>T1631.001</v>
+      </c>
+      <c r="B122" t="s">
+        <v>163</v>
+      </c>
+      <c r="C122" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A123" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1577/","T1577")</f>
+        <v>T1577</v>
+      </c>
+      <c r="B123" t="s">
+        <v>168</v>
+      </c>
+      <c r="C123" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A124" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1577/","T1577")</f>
+        <v>T1577</v>
+      </c>
+      <c r="B124" t="s">
+        <v>168</v>
+      </c>
+      <c r="C124" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A125" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1577/","T1577")</f>
+        <v>T1577</v>
+      </c>
+      <c r="B125" t="s">
+        <v>168</v>
+      </c>
+      <c r="C125" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A126" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1577/","T1577")</f>
+        <v>T1577</v>
+      </c>
+      <c r="B126" t="s">
+        <v>168</v>
+      </c>
+      <c r="C126" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A127" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1645/","T1645")</f>
+        <v>T1645</v>
+      </c>
+      <c r="B127" t="s">
+        <v>170</v>
+      </c>
+      <c r="C127" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A128" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1645/","T1645")</f>
+        <v>T1645</v>
+      </c>
+      <c r="B128" t="s">
+        <v>170</v>
+      </c>
+      <c r="C128" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A129" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1637/","T1637")</f>
+        <v>T1637</v>
+      </c>
+      <c r="B129" t="s">
+        <v>172</v>
+      </c>
+      <c r="C129" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A130" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1637/","T1637")</f>
+        <v>T1637</v>
+      </c>
+      <c r="B130" t="s">
+        <v>172</v>
+      </c>
+      <c r="C130" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A131" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1637/001/","T1637.001")</f>
+        <v>T1637.001</v>
+      </c>
+      <c r="B131" t="s">
+        <v>174</v>
+      </c>
+      <c r="C131" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A132" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1637/001/","T1637.001")</f>
+        <v>T1637.001</v>
+      </c>
+      <c r="B132" t="s">
+        <v>174</v>
+      </c>
+      <c r="C132" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A133" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1481/","T1481")</f>
+        <v>T1481</v>
+      </c>
+      <c r="B133" t="s">
+        <v>176</v>
+      </c>
+      <c r="C133" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A134" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1481/001/","T1481.001")</f>
+        <v>T1481.001</v>
+      </c>
+      <c r="B134" t="s">
+        <v>178</v>
+      </c>
+      <c r="C134" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A135" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1481/002/","T1481.002")</f>
+        <v>T1481.002</v>
+      </c>
+      <c r="B135" t="s">
+        <v>180</v>
+      </c>
+      <c r="C135" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A136" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1481/003/","T1481.003")</f>
+        <v>T1481.003</v>
+      </c>
+      <c r="B136" t="s">
+        <v>182</v>
+      </c>
+      <c r="C136" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A137" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1474/","T1474")</f>
+        <v>T1474</v>
+      </c>
+      <c r="B137" t="s">
+        <v>189</v>
+      </c>
+      <c r="C137" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A138" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1474/001/","T1474.001")</f>
+        <v>T1474.001</v>
+      </c>
+      <c r="B138" t="s">
+        <v>191</v>
+      </c>
+      <c r="C138" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A139" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1474/001/","T1474.001")</f>
+        <v>T1474.001</v>
+      </c>
+      <c r="B139" t="s">
+        <v>191</v>
+      </c>
+      <c r="C139" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A140" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1474/002/","T1474.002")</f>
+        <v>T1474.002</v>
+      </c>
+      <c r="B140" t="s">
+        <v>193</v>
+      </c>
+      <c r="C140" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A141" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1474/002/","T1474.002")</f>
+        <v>T1474.002</v>
+      </c>
+      <c r="B141" t="s">
+        <v>193</v>
+      </c>
+      <c r="C141" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A142" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1474/002/","T1474.002")</f>
+        <v>T1474.002</v>
+      </c>
+      <c r="B142" t="s">
+        <v>193</v>
+      </c>
+      <c r="C142" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A143" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1474/003/","T1474.003")</f>
+        <v>T1474.003</v>
+      </c>
+      <c r="B143" t="s">
+        <v>195</v>
+      </c>
+      <c r="C143" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A144" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1474/003/","T1474.003")</f>
+        <v>T1474.003</v>
+      </c>
+      <c r="B144" t="s">
+        <v>195</v>
+      </c>
+      <c r="C144" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A145" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1641/001/","T1641.001")</f>
+        <v>T1641.001</v>
+      </c>
+      <c r="B145" t="s">
+        <v>201</v>
+      </c>
+      <c r="C145" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A146" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1641/001/","T1641.001")</f>
+        <v>T1641.001</v>
+      </c>
+      <c r="B146" t="s">
+        <v>201</v>
+      </c>
+      <c r="C146" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A147" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1641/001/","T1641.001")</f>
+        <v>T1641.001</v>
+      </c>
+      <c r="B147" t="s">
+        <v>201</v>
+      </c>
+      <c r="C147" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A148" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1437/001/","T1437.001")</f>
+        <v>T1437.001</v>
+      </c>
+      <c r="B148" t="s">
+        <v>294</v>
+      </c>
+      <c r="C148" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A149" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1643/","T1643")</f>
+        <v>T1643</v>
+      </c>
+      <c r="B149" t="s">
+        <v>258</v>
+      </c>
+      <c r="C149" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A150" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1643/","T1643")</f>
+        <v>T1643</v>
+      </c>
+      <c r="B150" t="s">
+        <v>258</v>
+      </c>
+      <c r="C150" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A151" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1604/","T1604")</f>
+        <v>T1604</v>
+      </c>
+      <c r="B151" t="s">
+        <v>296</v>
+      </c>
+      <c r="C151" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A152" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1604/","T1604")</f>
+        <v>T1604</v>
+      </c>
+      <c r="B152" t="s">
+        <v>296</v>
+      </c>
+      <c r="C152" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A153" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1582/","T1582")</f>
+        <v>T1582</v>
+      </c>
+      <c r="B153" t="s">
+        <v>260</v>
+      </c>
+      <c r="C153" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A154" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1582/","T1582")</f>
+        <v>T1582</v>
+      </c>
+      <c r="B154" t="s">
+        <v>260</v>
+      </c>
+      <c r="C154" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A155" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1582/","T1582")</f>
+        <v>T1582</v>
+      </c>
+      <c r="B155" t="s">
+        <v>260</v>
+      </c>
+      <c r="C155" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A156" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1582/","T1582")</f>
+        <v>T1582</v>
+      </c>
+      <c r="B156" t="s">
+        <v>260</v>
+      </c>
+      <c r="C156" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A157" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1582/","T1582")</f>
+        <v>T1582</v>
+      </c>
+      <c r="B157" t="s">
+        <v>260</v>
+      </c>
+      <c r="C157" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A158" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1429/","T1429")</f>
+        <v>T1429</v>
+      </c>
+      <c r="B158" t="s">
+        <v>215</v>
+      </c>
+      <c r="C158" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A159" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1512/","T1512")</f>
+        <v>T1512</v>
+      </c>
+      <c r="B159" t="s">
+        <v>242</v>
+      </c>
+      <c r="C159" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A160" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1513/","T1513")</f>
+        <v>T1513</v>
+      </c>
+      <c r="B160" t="s">
+        <v>298</v>
+      </c>
+      <c r="C160" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A161" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1517/","T1517")</f>
+        <v>T1517</v>
+      </c>
+      <c r="B161" t="s">
+        <v>205</v>
+      </c>
+      <c r="C161" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A162" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1517/","T1517")</f>
+        <v>T1517</v>
+      </c>
+      <c r="B162" t="s">
+        <v>205</v>
+      </c>
+      <c r="C162" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A163" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1517/","T1517")</f>
+        <v>T1517</v>
+      </c>
+      <c r="B163" t="s">
+        <v>205</v>
+      </c>
+      <c r="C163" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A164" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1634/","T1634")</f>
+        <v>T1634</v>
+      </c>
+      <c r="B164" t="s">
+        <v>300</v>
+      </c>
+      <c r="C164" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A165" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1634/001/","T1634.001")</f>
+        <v>T1634.001</v>
+      </c>
+      <c r="B165" t="s">
+        <v>301</v>
+      </c>
+      <c r="C165" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A166" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1533/","T1533")</f>
+        <v>T1533</v>
+      </c>
+      <c r="B166" t="s">
+        <v>223</v>
+      </c>
+      <c r="C166" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A167" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1420/","T1420")</f>
+        <v>T1420</v>
+      </c>
+      <c r="B167" t="s">
+        <v>303</v>
+      </c>
+      <c r="C167" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A168" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1409/","T1409")</f>
+        <v>T1409</v>
+      </c>
+      <c r="B168" t="s">
+        <v>240</v>
+      </c>
+      <c r="C168" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A169" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1633/","T1633")</f>
+        <v>T1633</v>
+      </c>
+      <c r="B169" t="s">
+        <v>311</v>
+      </c>
+      <c r="C169" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A170" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1633/001/","T1633.001")</f>
+        <v>T1633.001</v>
+      </c>
+      <c r="B170" t="s">
+        <v>313</v>
+      </c>
+      <c r="C170" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A171" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1629/","T1629")</f>
+        <v>T1629</v>
+      </c>
+      <c r="B171" t="s">
+        <v>263</v>
+      </c>
+      <c r="C171" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A172" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1629/","T1629")</f>
+        <v>T1629</v>
+      </c>
+      <c r="B172" t="s">
+        <v>263</v>
+      </c>
+      <c r="C172" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A173" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1629/003/","T1629.003")</f>
+        <v>T1629.003</v>
+      </c>
+      <c r="B173" t="s">
+        <v>265</v>
+      </c>
+      <c r="C173" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A174" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1629/003/","T1629.003")</f>
+        <v>T1629.003</v>
+      </c>
+      <c r="B174" t="s">
+        <v>265</v>
+      </c>
+      <c r="C174" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A175" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1632/","T1632")</f>
+        <v>T1632</v>
+      </c>
+      <c r="B175" t="s">
+        <v>267</v>
+      </c>
+      <c r="C175" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A176" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1632/","T1632")</f>
+        <v>T1632</v>
+      </c>
+      <c r="B176" t="s">
+        <v>267</v>
+      </c>
+      <c r="C176" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A177" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1632/001/","T1632.001")</f>
+        <v>T1632.001</v>
+      </c>
+      <c r="B177" t="s">
+        <v>269</v>
+      </c>
+      <c r="C177" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A178" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1632/001/","T1632.001")</f>
+        <v>T1632.001</v>
+      </c>
+      <c r="B178" t="s">
+        <v>269</v>
+      </c>
+      <c r="C178" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A179" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1617/","T1617")</f>
+        <v>T1617</v>
+      </c>
+      <c r="B179" t="s">
+        <v>316</v>
+      </c>
+      <c r="C179" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A180" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1617/","T1617")</f>
+        <v>T1617</v>
+      </c>
+      <c r="B180" t="s">
+        <v>316</v>
+      </c>
+      <c r="C180" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A181" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/001/","T1630.001")</f>
+        <v>T1630.001</v>
+      </c>
+      <c r="B181" t="s">
+        <v>271</v>
+      </c>
+      <c r="C181" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A182" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/001/","T1630.001")</f>
+        <v>T1630.001</v>
+      </c>
+      <c r="B182" t="s">
+        <v>271</v>
+      </c>
+      <c r="C182" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A183" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/001/","T1630.001")</f>
+        <v>T1630.001</v>
+      </c>
+      <c r="B183" t="s">
+        <v>271</v>
+      </c>
+      <c r="C183" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A184" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/002/","T1630.002")</f>
+        <v>T1630.002</v>
+      </c>
+      <c r="B184" t="s">
+        <v>273</v>
+      </c>
+      <c r="C184" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A185" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/002/","T1630.002")</f>
+        <v>T1630.002</v>
+      </c>
+      <c r="B185" t="s">
+        <v>273</v>
+      </c>
+      <c r="C185" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A186" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/002/","T1630.002")</f>
+        <v>T1630.002</v>
+      </c>
+      <c r="B186" t="s">
+        <v>273</v>
+      </c>
+      <c r="C186" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A187" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/002/","T1630.002")</f>
+        <v>T1630.002</v>
+      </c>
+      <c r="B187" t="s">
+        <v>273</v>
+      </c>
+      <c r="C187" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A188" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/002/","T1630.002")</f>
+        <v>T1630.002</v>
+      </c>
+      <c r="B188" t="s">
+        <v>273</v>
+      </c>
+      <c r="C188" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A189" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/003/","T1630.003")</f>
+        <v>T1630.003</v>
+      </c>
+      <c r="B189" t="s">
+        <v>275</v>
+      </c>
+      <c r="C189" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A190" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/003/","T1630.003")</f>
+        <v>T1630.003</v>
+      </c>
+      <c r="B190" t="s">
+        <v>275</v>
+      </c>
+      <c r="C190" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A191" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1630/003/","T1630.003")</f>
+        <v>T1630.003</v>
+      </c>
+      <c r="B191" t="s">
+        <v>275</v>
+      </c>
+      <c r="C191" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A192" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1544/","T1544")</f>
+        <v>T1544</v>
+      </c>
+      <c r="B192" t="s">
+        <v>318</v>
+      </c>
+      <c r="C192" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A193" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1544/","T1544")</f>
+        <v>T1544</v>
+      </c>
+      <c r="B193" t="s">
+        <v>318</v>
+      </c>
+      <c r="C193" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A194" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1639/","T1639")</f>
+        <v>T1639</v>
+      </c>
+      <c r="B194" t="s">
+        <v>320</v>
+      </c>
+      <c r="C194" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A195" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1639/001/","T1639.001")</f>
+        <v>T1639.001</v>
+      </c>
+      <c r="B195" t="s">
+        <v>321</v>
+      </c>
+      <c r="C195" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A196" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1646/","T1646")</f>
+        <v>T1646</v>
+      </c>
+      <c r="B196" t="s">
+        <v>322</v>
+      </c>
+      <c r="C196" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A197" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1414/","T1414")</f>
+        <v>T1414</v>
+      </c>
+      <c r="B197" t="s">
+        <v>217</v>
+      </c>
+      <c r="C197" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A198" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1641/","T1641")</f>
+        <v>T1641</v>
+      </c>
+      <c r="B198" t="s">
+        <v>325</v>
+      </c>
+      <c r="C198" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A199" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1471/","T1471")</f>
+        <v>T1471</v>
+      </c>
+      <c r="B199" t="s">
+        <v>284</v>
+      </c>
+      <c r="C199" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A200" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1471/","T1471")</f>
+        <v>T1471</v>
+      </c>
+      <c r="B200" t="s">
+        <v>284</v>
+      </c>
+      <c r="C200" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A201" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1471/","T1471")</f>
+        <v>T1471</v>
+      </c>
+      <c r="B201" t="s">
+        <v>284</v>
+      </c>
+      <c r="C201" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A202" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1471/","T1471")</f>
+        <v>T1471</v>
+      </c>
+      <c r="B202" t="s">
+        <v>284</v>
+      </c>
+      <c r="C202" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A203" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1417/","T1417")</f>
+        <v>T1417</v>
+      </c>
+      <c r="B203" t="s">
+        <v>225</v>
+      </c>
+      <c r="C203" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A204" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1458/","T1458")</f>
+        <v>T1458</v>
+      </c>
+      <c r="B204" t="s">
+        <v>339</v>
+      </c>
+      <c r="C204" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A205" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1458/","T1458")</f>
+        <v>T1458</v>
+      </c>
+      <c r="B205" t="s">
+        <v>339</v>
+      </c>
+      <c r="C205" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A206" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1458/","T1458")</f>
+        <v>T1458</v>
+      </c>
+      <c r="B206" t="s">
+        <v>339</v>
+      </c>
+      <c r="C206" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A207" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1458/","T1458")</f>
+        <v>T1458</v>
+      </c>
+      <c r="B207" t="s">
+        <v>339</v>
+      </c>
+      <c r="C207" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A208" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1407/","T1407")</f>
+        <v>T1407</v>
+      </c>
+      <c r="B208" t="s">
+        <v>277</v>
+      </c>
+      <c r="C208" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A209" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1407/","T1407")</f>
+        <v>T1407</v>
+      </c>
+      <c r="B209" t="s">
+        <v>277</v>
+      </c>
+      <c r="C209" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A210" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1456/","T1456")</f>
+        <v>T1456</v>
+      </c>
+      <c r="B210" t="s">
+        <v>357</v>
+      </c>
+      <c r="C210" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A211" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1456/","T1456")</f>
+        <v>T1456</v>
+      </c>
+      <c r="B211" t="s">
+        <v>357</v>
+      </c>
+      <c r="C211" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A212" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1456/","T1456")</f>
+        <v>T1456</v>
+      </c>
+      <c r="B212" t="s">
+        <v>357</v>
+      </c>
+      <c r="C212" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A213" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1461/","T1461")</f>
+        <v>T1461</v>
+      </c>
+      <c r="B213" t="s">
+        <v>374</v>
+      </c>
+      <c r="C213" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A214" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1461/","T1461")</f>
+        <v>T1461</v>
+      </c>
+      <c r="B214" t="s">
+        <v>374</v>
+      </c>
+      <c r="C214" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A215" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1616/","T1616")</f>
+        <v>T1616</v>
+      </c>
+      <c r="B215" t="s">
+        <v>250</v>
+      </c>
+      <c r="C215" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A216" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1616/","T1616")</f>
+        <v>T1616</v>
+      </c>
+      <c r="B216" t="s">
+        <v>250</v>
+      </c>
+      <c r="C216" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A217" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1616/","T1616")</f>
+        <v>T1616</v>
+      </c>
+      <c r="B217" t="s">
+        <v>250</v>
+      </c>
+      <c r="C217" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A218" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1575/","T1575")</f>
+        <v>T1575</v>
+      </c>
+      <c r="B218" t="s">
+        <v>401</v>
+      </c>
+      <c r="C218" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A219" t="str">
+        <f>HYPERLINK("https://attack.mitre.org/techniques/T1635/","T1635")</f>
+        <v>T1635</v>
+      </c>
+      <c r="B219" t="s">
+        <v>207</v>
+      </c>
+      <c r="C219" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="312" ht="15.5" x14ac:dyDescent="0.35"/>
@@ -2725,7 +5540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7AF39-A8AE-1448-8EA3-B969364DCC63}">
   <dimension ref="A1:XFD155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
@@ -39630,15 +42445,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Date_x0020__x0026__x0020_Time xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
@@ -39655,6 +42461,15 @@
     <CostPer xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -39957,20 +42772,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CF67D68-5D9D-4184-8FCF-9F43A8746F62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B241570-251F-4639-B053-9597F90135CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="0ca01121-da18-407e-86a0-e0ab1b6c7d8c"/>
     <ds:schemaRef ds:uri="ec3e3de1-934b-464b-893a-587ae869df79"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CF67D68-5D9D-4184-8FCF-9F43A8746F62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>